<commit_message>
Add semaphore-nt test and update benchmark results
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\CORENTINE\VDI\ALUMNO\dagapas\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neko\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7738C6BA-C74B-44CA-9DBC-D3260B73045A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9B55C9-40AF-40FA-91D1-865A53844E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F08F9825-9BEF-4EE3-B725-D8DD9B73E4C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F08F9825-9BEF-4EE3-B725-D8DD9B73E4C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Rewrites</t>
   </si>
@@ -81,15 +91,6 @@
     <t>STRASS:</t>
   </si>
   <si>
-    <t>Only ATAME</t>
-  </si>
-  <si>
-    <t>Only STRASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Max %</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -100,16 +101,29 @@
   </si>
   <si>
     <t>Result diff.</t>
+  </si>
+  <si>
+    <t>Absolute</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>SEMAPHORE-NT</t>
+  </si>
+  <si>
+    <t>false || 0 || p 1 {idle} p 2 {idle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -359,19 +373,6 @@
       <right style="thin">
         <color rgb="FF7F7F7F"/>
       </right>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -404,7 +405,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thick">
         <color theme="4" tint="0.499984740745262"/>
       </top>
@@ -415,12 +418,95 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -434,7 +520,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -444,29 +530,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,44 +569,63 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="9" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="19" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="21" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Entrada" xfId="3" builtinId="20"/>
@@ -905,16 +1017,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121D382F-F2C4-47BA-B9B1-3F8C4317679B}">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="32" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="1"/>
     <col min="5" max="6" width="11.42578125" style="8"/>
     <col min="7" max="7" width="11.42578125" style="2"/>
@@ -922,46 +1034,44 @@
     <col min="11" max="11" width="11.42578125" style="2"/>
     <col min="13" max="13" width="11.42578125" style="2"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" thickBot="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="21"/>
+      <c r="N1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="37"/>
-      <c r="P1" s="38"/>
+      <c r="O1" s="19"/>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="19"/>
+    <row r="2" spans="1:18" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
@@ -992,418 +1102,635 @@
       <c r="M2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="22" t="s">
+      <c r="N2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="C3" s="13">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="29">
+        <v>1861</v>
+      </c>
+      <c r="E3" s="53">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F3" s="53">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>42295</v>
+      </c>
+      <c r="H3" s="29">
+        <v>374472</v>
+      </c>
+      <c r="I3" s="53">
+        <v>0.06</v>
+      </c>
+      <c r="J3" s="53">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6241200</v>
+      </c>
+      <c r="L3" s="29">
+        <f t="shared" ref="L3" si="0">E3/I3</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ref="M3" si="1">F3/J3</f>
+        <v>0.72131147540983609</v>
+      </c>
+      <c r="N3" s="32">
+        <v>13</v>
+      </c>
+      <c r="O3" s="16">
+        <f>$N3/$C3</f>
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="13">
+        <v>100000</v>
+      </c>
+      <c r="D4" s="29">
+        <v>198845</v>
+      </c>
+      <c r="E4" s="53">
+        <v>33.911999999999999</v>
+      </c>
+      <c r="F4" s="53">
+        <v>33.914000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5863</v>
+      </c>
+      <c r="H4" s="29">
+        <v>37088928</v>
+      </c>
+      <c r="I4" s="53">
+        <v>25.596</v>
+      </c>
+      <c r="J4" s="53">
+        <v>25.597000000000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1449012</v>
+      </c>
+      <c r="L4" s="29">
+        <f t="shared" ref="L4:M14" si="2">E4/I4</f>
+        <v>1.3248945147679325</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3249208891666993</v>
+      </c>
+      <c r="N4" s="32">
+        <v>1124</v>
+      </c>
+      <c r="O4" s="16">
+        <f>$N4/$C4</f>
+        <v>1.124E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35">
+        <v>500000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>996674</v>
+      </c>
+      <c r="E5" s="54">
+        <v>419.22</v>
+      </c>
+      <c r="F5" s="54">
+        <v>419.21699999999998</v>
+      </c>
+      <c r="G5" s="36">
+        <v>2377</v>
+      </c>
+      <c r="H5" s="37">
+        <v>185440516</v>
+      </c>
+      <c r="I5" s="56">
+        <v>272.96800000000002</v>
+      </c>
+      <c r="J5" s="56">
+        <v>272.96699999999998</v>
+      </c>
+      <c r="K5" s="36">
+        <v>679348</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5357844142903196</v>
+      </c>
+      <c r="M5" s="36">
+        <f t="shared" si="2"/>
+        <v>1.5357790502148612</v>
+      </c>
+      <c r="N5" s="38">
+        <v>5549</v>
+      </c>
+      <c r="O5" s="39">
+        <f t="shared" ref="O5:O14" si="3">$N5/$C5</f>
+        <v>1.1098E-2</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="43">
+        <v>1805</v>
+      </c>
+      <c r="E6" s="55">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F6" s="55">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G6" s="44">
+        <v>50138</v>
+      </c>
+      <c r="H6" s="43">
+        <v>256192</v>
+      </c>
+      <c r="I6" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="J6" s="55">
+        <v>0.04</v>
+      </c>
+      <c r="K6" s="44">
+        <v>6404800</v>
+      </c>
+      <c r="L6" s="43">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="M6" s="44">
+        <f t="shared" si="2"/>
+        <v>0.92499999999999993</v>
+      </c>
+      <c r="N6" s="45">
+        <v>134</v>
+      </c>
+      <c r="O6" s="46">
+        <f t="shared" si="3"/>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="12">
+        <v>100000</v>
+      </c>
+      <c r="D7" s="29">
+        <v>247281</v>
+      </c>
+      <c r="E7" s="53">
+        <v>9.5960000000000001</v>
+      </c>
+      <c r="F7" s="53">
+        <v>9.5950000000000006</v>
+      </c>
+      <c r="G7" s="2">
+        <v>25769</v>
+      </c>
+      <c r="H7" s="6">
+        <v>22110204</v>
+      </c>
+      <c r="I7" s="57">
+        <v>8.0640000000000001</v>
+      </c>
+      <c r="J7" s="57">
+        <v>8.0619999999999994</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2741840</v>
+      </c>
+      <c r="L7" s="29">
+        <f t="shared" si="2"/>
+        <v>1.1899801587301588</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1901513272140909</v>
+      </c>
+      <c r="N7" s="32">
+        <v>1940</v>
+      </c>
+      <c r="O7" s="16">
+        <f t="shared" si="3"/>
+        <v>1.9400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="35">
+        <v>500000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1264328</v>
+      </c>
+      <c r="E8" s="54">
+        <v>84.688000000000002</v>
+      </c>
+      <c r="F8" s="54">
+        <v>84.686999999999998</v>
+      </c>
+      <c r="G8" s="36">
+        <v>14929</v>
+      </c>
+      <c r="H8" s="37">
+        <v>109884763</v>
+      </c>
+      <c r="I8" s="56">
+        <v>60.683999999999997</v>
+      </c>
+      <c r="J8" s="56">
+        <v>60.686</v>
+      </c>
+      <c r="K8" s="36">
+        <v>1810769</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="2"/>
+        <v>1.3955573132951027</v>
+      </c>
+      <c r="M8" s="36">
+        <f t="shared" si="2"/>
+        <v>1.3954948423030022</v>
+      </c>
+      <c r="N8" s="38">
+        <v>6473</v>
+      </c>
+      <c r="O8" s="39">
+        <f t="shared" si="3"/>
+        <v>1.2945999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>20</v>
       </c>
+      <c r="C9" s="42">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="43">
+        <v>88042</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="G9" s="44">
+        <v>132593</v>
+      </c>
+      <c r="H9" s="48">
+        <v>2135496</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="J9" s="55">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K9" s="44">
+        <v>2311142</v>
+      </c>
+      <c r="L9" s="43">
+        <f t="shared" si="2"/>
+        <v>0.7186147186147186</v>
+      </c>
+      <c r="M9" s="44">
+        <f t="shared" si="2"/>
+        <v>0.71459459459459462</v>
+      </c>
+      <c r="N9" s="45">
+        <v>907</v>
+      </c>
+      <c r="O9" s="46">
+        <f t="shared" si="3"/>
+        <v>9.0700000000000003E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="49">
+        <v>13783</v>
+      </c>
+      <c r="D10" s="3">
+        <v>147197</v>
+      </c>
+      <c r="E10" s="54">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="F10" s="54">
+        <v>1.101</v>
+      </c>
+      <c r="G10" s="36">
+        <v>133330</v>
+      </c>
+      <c r="H10" s="37">
+        <v>2970250</v>
+      </c>
+      <c r="I10" s="54">
+        <v>1.264</v>
+      </c>
+      <c r="J10" s="54">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="K10" s="36">
+        <v>2349881</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87341772151898744</v>
+      </c>
+      <c r="M10" s="36">
+        <f t="shared" si="2"/>
+        <v>0.87311657414750199</v>
+      </c>
+      <c r="N10" s="38">
+        <v>0</v>
+      </c>
+      <c r="O10" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="42">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="43">
+        <v>2330</v>
+      </c>
+      <c r="E11" s="55">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F11" s="55">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G11" s="44">
+        <v>278000</v>
+      </c>
+      <c r="H11" s="48">
+        <v>3336</v>
+      </c>
+      <c r="I11" s="55">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J11" s="55">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K11" s="44">
+        <v>278000</v>
+      </c>
+      <c r="L11" s="43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="44">
+        <f t="shared" si="2"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="N11" s="32">
+        <v>0</v>
+      </c>
+      <c r="O11" s="46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="12">
         <v>100000</v>
       </c>
-      <c r="D3">
-        <v>198845</v>
-      </c>
-      <c r="E3" s="8">
-        <v>33.911999999999999</v>
-      </c>
-      <c r="F3" s="8">
-        <v>33.914000000000001</v>
-      </c>
-      <c r="G3" s="2">
-        <v>5863</v>
-      </c>
-      <c r="H3">
-        <v>37088928</v>
-      </c>
-      <c r="I3" s="8">
-        <v>25.596</v>
-      </c>
-      <c r="J3" s="8">
-        <v>25.597000000000001</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1449012</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:M9" si="0">E3/I3</f>
-        <v>1.3248945147679325</v>
-      </c>
-      <c r="M3" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3249208891666993</v>
-      </c>
-      <c r="N3" s="23">
-        <v>1124</v>
-      </c>
-      <c r="O3" s="23">
-        <v>1124</v>
-      </c>
-      <c r="P3" s="34">
-        <f>MAX($N3/$C3,$O3/$C3)</f>
-        <v>1.124E-2</v>
+      <c r="D12" s="6">
+        <v>233330</v>
+      </c>
+      <c r="E12" s="53">
+        <v>1.3080000000000001</v>
+      </c>
+      <c r="F12" s="53">
+        <v>1.3080000000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>178386</v>
+      </c>
+      <c r="H12" s="6">
+        <v>333336</v>
+      </c>
+      <c r="I12" s="53">
+        <v>1.48</v>
+      </c>
+      <c r="J12" s="53">
+        <v>1.482</v>
+      </c>
+      <c r="K12" s="2">
+        <v>225227</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="2"/>
+        <v>0.88378378378378386</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.88259109311740891</v>
+      </c>
+      <c r="N12" s="32">
+        <v>0</v>
+      </c>
+      <c r="O12" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="15"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="24">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="12">
         <v>500000</v>
       </c>
-      <c r="D4">
-        <v>996674</v>
-      </c>
-      <c r="E4" s="8">
-        <v>419.22</v>
-      </c>
-      <c r="F4" s="8">
-        <v>419.21699999999998</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2377</v>
-      </c>
-      <c r="H4" s="6">
-        <v>185440516</v>
-      </c>
-      <c r="I4" s="9">
-        <v>272.96800000000002</v>
-      </c>
-      <c r="J4" s="9">
-        <v>272.96699999999998</v>
-      </c>
-      <c r="K4" s="2">
-        <v>679348</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>1.5357844142903196</v>
-      </c>
-      <c r="M4" s="2">
-        <f t="shared" si="0"/>
-        <v>1.5357790502148612</v>
-      </c>
-      <c r="N4" s="23">
-        <v>5549</v>
-      </c>
-      <c r="O4" s="23">
-        <v>5549</v>
-      </c>
-      <c r="P4" s="34">
-        <f t="shared" ref="P4:P9" si="1">MAX($N4/$C4,$O4/$C4)</f>
-        <v>1.1098E-2</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>14</v>
+      <c r="D13" s="29">
+        <v>1166662</v>
+      </c>
+      <c r="E13" s="53">
+        <v>14.584</v>
+      </c>
+      <c r="F13" s="53">
+        <v>14.584</v>
+      </c>
+      <c r="G13" s="2">
+        <v>79996</v>
+      </c>
+      <c r="H13" s="29">
+        <v>1666670</v>
+      </c>
+      <c r="I13" s="53">
+        <v>10.46</v>
+      </c>
+      <c r="J13" s="53">
+        <v>10.457000000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <v>159337</v>
+      </c>
+      <c r="L13" s="29">
+        <f t="shared" ref="L13" si="4">E13/I13</f>
+        <v>1.3942638623326957</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" ref="M13" si="5">F13/J13</f>
+        <v>1.3946638615281628</v>
+      </c>
+      <c r="N13" s="32">
+        <v>0</v>
+      </c>
+      <c r="O13" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="24">
-        <v>1000</v>
-      </c>
-      <c r="D5">
-        <v>1805</v>
-      </c>
-      <c r="E5" s="8">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="F5" s="8">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="G5" s="2">
-        <v>50138</v>
-      </c>
-      <c r="H5">
-        <v>256192</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="K5" s="2">
-        <v>6404800</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="M5" s="2">
-        <f t="shared" si="0"/>
-        <v>0.92499999999999993</v>
-      </c>
-      <c r="N5" s="23">
-        <v>134</v>
-      </c>
-      <c r="O5" s="23">
-        <v>134</v>
-      </c>
-      <c r="P5" s="34">
-        <f t="shared" si="1"/>
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>15</v>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35">
+        <v>1000000</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2333330</v>
+      </c>
+      <c r="E14" s="54">
+        <v>47.643999999999998</v>
+      </c>
+      <c r="F14" s="54">
+        <v>47.646000000000001</v>
+      </c>
+      <c r="G14" s="36">
+        <v>48974</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3333336</v>
+      </c>
+      <c r="I14" s="54">
+        <v>27.988</v>
+      </c>
+      <c r="J14" s="54">
+        <v>27.988</v>
+      </c>
+      <c r="K14" s="36">
+        <v>119098</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7023009861369158</v>
+      </c>
+      <c r="M14" s="36">
+        <f t="shared" si="2"/>
+        <v>1.7023724453337146</v>
+      </c>
+      <c r="N14" s="58">
+        <v>0</v>
+      </c>
+      <c r="O14" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="17"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="24">
-        <v>100000</v>
-      </c>
-      <c r="D6">
-        <v>247281</v>
-      </c>
-      <c r="E6" s="8">
-        <v>9.5960000000000001</v>
-      </c>
-      <c r="F6" s="8">
-        <v>9.5950000000000006</v>
-      </c>
-      <c r="G6" s="2">
-        <v>25769</v>
-      </c>
-      <c r="H6" s="6">
-        <v>22110204</v>
-      </c>
-      <c r="I6" s="9">
-        <v>8.0640000000000001</v>
-      </c>
-      <c r="J6" s="9">
-        <v>8.0619999999999994</v>
-      </c>
-      <c r="K6" s="2">
-        <v>2741840</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>1.1899801587301588</v>
-      </c>
-      <c r="M6" s="2">
-        <f t="shared" si="0"/>
-        <v>1.1901513272140909</v>
-      </c>
-      <c r="N6" s="23">
-        <v>1940</v>
-      </c>
-      <c r="O6" s="23">
-        <v>1940</v>
-      </c>
-      <c r="P6" s="34">
-        <f t="shared" si="1"/>
-        <v>1.9400000000000001E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="15"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="24">
-        <v>500000</v>
-      </c>
-      <c r="D7">
-        <v>1264328</v>
-      </c>
-      <c r="E7" s="8">
-        <v>84.688000000000002</v>
-      </c>
-      <c r="F7" s="8">
-        <v>84.686999999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>14929</v>
-      </c>
-      <c r="H7" s="6">
-        <v>109884763</v>
-      </c>
-      <c r="I7" s="9">
-        <v>60.683999999999997</v>
-      </c>
-      <c r="J7" s="9">
-        <v>60.686</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1810769</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>1.3955573132951027</v>
-      </c>
-      <c r="M7" s="2">
-        <f t="shared" si="0"/>
-        <v>1.3954948423030022</v>
-      </c>
-      <c r="N7" s="23">
-        <v>6473</v>
-      </c>
-      <c r="O7" s="23">
-        <v>6473</v>
-      </c>
-      <c r="P7" s="34">
-        <f t="shared" si="1"/>
-        <v>1.2945999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="24">
-        <v>10000</v>
-      </c>
-      <c r="D8">
-        <v>88042</v>
-      </c>
-      <c r="E8" s="8">
-        <v>0.66400000000000003</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="G8" s="2">
-        <v>132593</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2135496</v>
-      </c>
-      <c r="I8" s="8">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="J8" s="8">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="K8" s="2">
-        <v>2311142</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>0.7186147186147186</v>
-      </c>
-      <c r="M8" s="2">
-        <f t="shared" si="0"/>
-        <v>0.71459459459459462</v>
-      </c>
-      <c r="N8" s="23">
-        <v>907</v>
-      </c>
-      <c r="O8" s="23">
-        <v>907</v>
-      </c>
-      <c r="P8" s="34">
-        <f t="shared" si="1"/>
-        <v>9.0700000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="15"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="26">
-        <v>13783</v>
-      </c>
-      <c r="D9">
-        <v>147197</v>
-      </c>
-      <c r="E9" s="8">
-        <v>1.1040000000000001</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1.101</v>
-      </c>
-      <c r="G9" s="2">
-        <v>133330</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2970250</v>
-      </c>
-      <c r="I9" s="8">
-        <v>1.264</v>
-      </c>
-      <c r="J9" s="8">
-        <v>1.2609999999999999</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2349881</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>0.87341772151898744</v>
-      </c>
-      <c r="M9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.87311657414750199</v>
-      </c>
-      <c r="N9" s="23">
-        <v>0</v>
-      </c>
-      <c r="O9" s="23">
-        <v>0</v>
-      </c>
-      <c r="P9" s="35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A8:A9"/>
+  <mergeCells count="15">
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:M1048576">
-    <cfRule type="top10" dxfId="4" priority="3" percent="1" rank="10"/>
-    <cfRule type="top10" dxfId="3" priority="4" percent="1" bottom="1" rank="10"/>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="greaterThan">
+    <cfRule type="top10" dxfId="4" priority="10" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="11" percent="1" bottom="1" rank="10"/>
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:M1048576">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="O3:O1048576">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="percentile" val="10"/>
         <cfvo type="percentile" val="50"/>
@@ -1413,7 +1740,7 @@
         <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>